<commit_message>
update to add column header values
</commit_message>
<xml_diff>
--- a/propub_variables.xlsx
+++ b/propub_variables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22918"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kindaran\Documents\upwork\Propublica interface\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A8453B-B4D6-462E-805A-3FCF9C52EBD6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C4014B3-EECD-4103-834C-C5E24736DB7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sample data" sheetId="1" r:id="rId2"/>
     <sheet name="API documentation" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +35,223 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="108">
+  <si>
+    <t>EINS</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>HeaderVar</t>
+  </si>
+  <si>
+    <t>FilingVar</t>
+  </si>
+  <si>
+    <t>FileHeader</t>
+  </si>
+  <si>
+    <t>ein</t>
+  </si>
+  <si>
+    <t>tax_prd</t>
+  </si>
+  <si>
+    <t>EIN</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>tax_prd_yr</t>
+  </si>
+  <si>
+    <t>Entity Name</t>
+  </si>
+  <si>
+    <t>BusinessNameLine1Txt</t>
+  </si>
+  <si>
+    <t>tax_period</t>
+  </si>
+  <si>
+    <t>totcntrbgfts</t>
+  </si>
+  <si>
+    <t>Tax Period</t>
+  </si>
+  <si>
+    <t>TaxYr</t>
+  </si>
+  <si>
+    <t>income_amount</t>
+  </si>
+  <si>
+    <t>totprgmrevnue</t>
+  </si>
+  <si>
+    <t>Investment Income</t>
+  </si>
+  <si>
+    <t>TaxPeriodEndDt</t>
+  </si>
+  <si>
+    <t>revenue_amount</t>
+  </si>
+  <si>
+    <t>invstmntinc</t>
+  </si>
+  <si>
+    <t>Total Revenue</t>
+  </si>
+  <si>
+    <t>TotalGrossUBIAmt</t>
+  </si>
+  <si>
+    <t>Fiscal Year</t>
+  </si>
+  <si>
+    <t>NetUnrelatedBusTxblIncmAmt</t>
+  </si>
+  <si>
+    <t>Fiscal Year End</t>
+  </si>
+  <si>
+    <t>CYContributionsGrantsAmt</t>
+  </si>
+  <si>
+    <t>Contributions And Grants</t>
+  </si>
+  <si>
+    <t>TotalProgramServiceRevenueAmt</t>
+  </si>
+  <si>
+    <t>Program Service Revenue</t>
+  </si>
+  <si>
+    <t>CYInvestmentIncomeAmt</t>
+  </si>
+  <si>
+    <t>CYOtherRevenueAmt</t>
+  </si>
+  <si>
+    <t>CYTotalRevenueAmt</t>
+  </si>
+  <si>
+    <t>TotalRevenueColumnAmt</t>
+  </si>
+  <si>
+    <t>CYGrantsAndSimilarPaidAmt</t>
+  </si>
+  <si>
+    <t>CYBenefitsPaidToMembersAmt</t>
+  </si>
+  <si>
+    <t>CYSalariesCompEmpBnftPaidAmt</t>
+  </si>
+  <si>
+    <t>CYTotalProfFndrsngExpnsAmt</t>
+  </si>
+  <si>
+    <t>CYOtherExpensesAmt</t>
+  </si>
+  <si>
+    <t>CYTotalExpensesAmt</t>
+  </si>
+  <si>
+    <t>LandBldgEquipBasisNetGrp</t>
+  </si>
+  <si>
+    <t>InvestmentsPubTradedSecGrp</t>
+  </si>
+  <si>
+    <t>InvestmentsOtherSecuritiesGrp</t>
+  </si>
+  <si>
+    <t>InvestmentsProgramRelatedGrp</t>
+  </si>
+  <si>
+    <t>TotalAssetsGrp</t>
+  </si>
+  <si>
+    <t>BookValueAmt</t>
+  </si>
+  <si>
+    <t>TotalLiabilitiesEOYAmt</t>
+  </si>
+  <si>
+    <t>BeginningYearBalanceAmt</t>
+  </si>
+  <si>
+    <t>ContributionsAmt</t>
+  </si>
+  <si>
+    <t>InvestmentEarningsOrLossesAmt</t>
+  </si>
+  <si>
+    <t>GrantsOrScholarshipsAmt</t>
+  </si>
+  <si>
+    <t>OtherExpendituresAmt</t>
+  </si>
+  <si>
+    <t>AdministrativeExpensesAmt</t>
+  </si>
+  <si>
+    <t>EndYearBalanceAmt</t>
+  </si>
+  <si>
+    <t>Sample XML form: https://s3.amazonaws.com/irs-form-990/201931299349301613_public.xml?_ga=2.109548227.757672968.1589333782-1715030194.1589333782</t>
+  </si>
+  <si>
+    <t>Sample document: https://projects.propublica.org/nonprofits/display_990/42103580/05_2019_prefixes_01-04%2F042103580_201806_990_2019052316338984</t>
+  </si>
+  <si>
+    <t>DESCRIPTION OF ENTITY</t>
+  </si>
+  <si>
+    <t>UNRELATED REVENUE</t>
+  </si>
+  <si>
+    <t>REVENUE</t>
+  </si>
+  <si>
+    <t>PROGRAM SERVICE REVENUE</t>
+  </si>
+  <si>
+    <t>INVESTMENT INCOME</t>
+  </si>
+  <si>
+    <t>EXPENSES</t>
+  </si>
+  <si>
+    <t>ASSETS</t>
+  </si>
+  <si>
+    <t>INVESTMENTS - OTHER SECURITIES</t>
+  </si>
+  <si>
+    <t>LIABILITIES</t>
+  </si>
+  <si>
+    <t>ENDOWMENT</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Variable modifier</t>
+  </si>
+  <si>
+    <t>EOYAmt</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Entity name</t>
+  </si>
   <si>
     <t>Filing year</t>
   </si>
@@ -41,302 +259,113 @@
     <t>Fiscal year end date</t>
   </si>
   <si>
-    <t>Entity name</t>
+    <t>Total unrelated business revenue</t>
+  </si>
+  <si>
+    <t>Net unrelated business taxable income</t>
+  </si>
+  <si>
+    <t>Contributions and grants</t>
+  </si>
+  <si>
+    <t>Program service revenue</t>
+  </si>
+  <si>
+    <t>Investment income</t>
+  </si>
+  <si>
+    <t>Other revenue</t>
+  </si>
+  <si>
+    <t>Total revenue</t>
+  </si>
+  <si>
+    <t>Student tuition, room and board</t>
+  </si>
+  <si>
+    <t>Investment income (including dividends, interest, and other similar amounts)</t>
+  </si>
+  <si>
+    <t>Net gain or loss from sales of assets other than inventory</t>
+  </si>
+  <si>
+    <t>Grants or similar amounts paid</t>
+  </si>
+  <si>
+    <t>Benefits paid to members</t>
+  </si>
+  <si>
+    <t>Salaries, other comp, employee benefits</t>
+  </si>
+  <si>
+    <t>Professional fundraising fees</t>
+  </si>
+  <si>
+    <t>Other expenses</t>
+  </si>
+  <si>
+    <t>Total expenses</t>
+  </si>
+  <si>
+    <t>Net land</t>
+  </si>
+  <si>
+    <t>Investments - publicly traded securities</t>
+  </si>
+  <si>
+    <t>Investments - other securities</t>
+  </si>
+  <si>
+    <t>Investments - program-related</t>
+  </si>
+  <si>
+    <t>Total assets</t>
+  </si>
+  <si>
+    <t>Real assets</t>
+  </si>
+  <si>
+    <t>Private equities</t>
+  </si>
+  <si>
+    <t>Total liabilities</t>
+  </si>
+  <si>
+    <t>Beginning of year</t>
+  </si>
+  <si>
+    <t>Contributions</t>
+  </si>
+  <si>
+    <t>Net investment earnings, gains and losses</t>
+  </si>
+  <si>
+    <t>Grants or scholarships</t>
+  </si>
+  <si>
+    <t>Other expenditures for facilities and programs</t>
+  </si>
+  <si>
+    <t>Administrative expenses</t>
+  </si>
+  <si>
+    <t>End of year balance</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
   <si>
     <t>PRESIDENT AND FELLOWS OF HARVARD COLLEGE</t>
   </si>
   <si>
-    <t>Total unrelated business revenue</t>
-  </si>
-  <si>
-    <t>Contributions and grants</t>
-  </si>
-  <si>
-    <t>Program service revenue</t>
-  </si>
-  <si>
-    <t>Investment income</t>
-  </si>
-  <si>
-    <t>Total revenue</t>
-  </si>
-  <si>
-    <t>REVENUE</t>
-  </si>
-  <si>
-    <t>Other revenue</t>
-  </si>
-  <si>
-    <t>EXPENSES</t>
-  </si>
-  <si>
-    <t>Benefits paid to members</t>
-  </si>
-  <si>
-    <t>Salaries, other comp, employee benefits</t>
-  </si>
-  <si>
-    <t>Professional fundraising fees</t>
-  </si>
-  <si>
-    <t>Other expenses</t>
-  </si>
-  <si>
-    <t>Total expenses</t>
-  </si>
-  <si>
-    <t>Grants or similar amounts paid</t>
-  </si>
-  <si>
-    <t>Student tuition, room and board</t>
-  </si>
-  <si>
-    <t>Net gain or loss from sales of assets other than inventory</t>
-  </si>
-  <si>
-    <t>Investment income (including dividends, interest, and other similar amounts)</t>
-  </si>
-  <si>
-    <t>ASSETS</t>
-  </si>
-  <si>
-    <t>Net land</t>
-  </si>
-  <si>
-    <t>Investments - publicly traded securities</t>
-  </si>
-  <si>
-    <t>Investments - other securities</t>
-  </si>
-  <si>
-    <t>Investments - program-related</t>
-  </si>
-  <si>
-    <t>Total assets</t>
-  </si>
-  <si>
-    <t>LIABILITIES</t>
-  </si>
-  <si>
-    <t>Total liabilities</t>
-  </si>
-  <si>
-    <t>Private equities</t>
-  </si>
-  <si>
-    <t>Real assets</t>
-  </si>
-  <si>
-    <t>Beginning of year</t>
-  </si>
-  <si>
-    <t>Contributions</t>
-  </si>
-  <si>
-    <t>Net investment earnings, gains and losses</t>
-  </si>
-  <si>
-    <t>Grants or scholarships</t>
-  </si>
-  <si>
-    <t>Other expenditures for facilities and programs</t>
-  </si>
-  <si>
-    <t>Administrative expenses</t>
-  </si>
-  <si>
-    <t>End of year balance</t>
-  </si>
-  <si>
-    <t>BeginningYearBalanceAmt</t>
-  </si>
-  <si>
-    <t>ContributionsAmt</t>
-  </si>
-  <si>
-    <t>InvestmentEarningsOrLossesAmt</t>
-  </si>
-  <si>
-    <t>GrantsOrScholarshipsAmt</t>
-  </si>
-  <si>
-    <t>AdministrativeExpensesAmt</t>
-  </si>
-  <si>
-    <t>OtherExpendituresAmt</t>
-  </si>
-  <si>
-    <t>EndYearBalanceAmt</t>
-  </si>
-  <si>
-    <t>ENDOWMENT</t>
-  </si>
-  <si>
-    <t>EIN</t>
-  </si>
-  <si>
-    <t>BusinessNameLine1Txt</t>
-  </si>
-  <si>
-    <t>TaxPeriodEndDt</t>
-  </si>
-  <si>
-    <t>TaxYr</t>
-  </si>
-  <si>
-    <t>TotalGrossUBIAmt</t>
-  </si>
-  <si>
-    <t>NetUnrelatedBusTxblIncmAmt</t>
-  </si>
-  <si>
-    <t>CYContributionsGrantsAmt</t>
-  </si>
-  <si>
-    <t>TotalProgramServiceRevenueAmt</t>
-  </si>
-  <si>
-    <t>CYInvestmentIncomeAmt</t>
-  </si>
-  <si>
-    <t>CYOtherRevenueAmt</t>
-  </si>
-  <si>
-    <t>CYTotalRevenueAmt</t>
-  </si>
-  <si>
-    <t>TotalRevenueColumnAmt</t>
-  </si>
-  <si>
-    <t>CYGrantsAndSimilarPaidAmt</t>
-  </si>
-  <si>
-    <t>CYSalariesCompEmpBnftPaidAmt</t>
-  </si>
-  <si>
-    <t>CYBenefitsPaidToMembersAmt</t>
-  </si>
-  <si>
-    <t>CYTotalProfFndrsngExpnsAmt</t>
-  </si>
-  <si>
-    <t>CYOtherExpensesAmt</t>
-  </si>
-  <si>
-    <t>CYTotalExpensesAmt</t>
-  </si>
-  <si>
-    <t>EOYAmt</t>
-  </si>
-  <si>
-    <t>LandBldgEquipBasisNetGrp</t>
-  </si>
-  <si>
-    <t>InvestmentsPubTradedSecGrp</t>
-  </si>
-  <si>
-    <t>InvestmentsOtherSecuritiesGrp</t>
-  </si>
-  <si>
-    <t>InvestmentsProgramRelatedGrp</t>
-  </si>
-  <si>
-    <t>TotalAssetsGrp</t>
-  </si>
-  <si>
-    <t>BookValueAmt</t>
-  </si>
-  <si>
-    <t>TotalLiabilitiesEOYAmt</t>
-  </si>
-  <si>
-    <t>DESCRIPTION OF ENTITY</t>
-  </si>
-  <si>
-    <t>Variable</t>
-  </si>
-  <si>
-    <t>Label</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Net unrelated business taxable income</t>
-  </si>
-  <si>
-    <t>UNRELATED REVENUE</t>
-  </si>
-  <si>
-    <t>PROGRAM SERVICE REVENUE</t>
-  </si>
-  <si>
-    <t>INVESTMENT INCOME</t>
-  </si>
-  <si>
-    <t>INVESTMENTS - OTHER SECURITIES</t>
-  </si>
-  <si>
-    <t>Variable modifier</t>
-  </si>
-  <si>
-    <t>Years</t>
-  </si>
-  <si>
-    <t>EINS</t>
-  </si>
-  <si>
-    <t>Sample XML form: https://s3.amazonaws.com/irs-form-990/201931299349301613_public.xml?_ga=2.109548227.757672968.1589333782-1715030194.1589333782</t>
-  </si>
-  <si>
     <t>https://projects.propublica.org/nonprofits/api</t>
-  </si>
-  <si>
-    <t>Sample document: https://projects.propublica.org/nonprofits/display_990/42103580/05_2019_prefixes_01-04%2F042103580_201806_990_2019052316338984</t>
-  </si>
-  <si>
-    <t>HeaderVar</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>ein</t>
-  </si>
-  <si>
-    <t>income_amount</t>
-  </si>
-  <si>
-    <t>revenue_amount</t>
-  </si>
-  <si>
-    <t>tax_period</t>
-  </si>
-  <si>
-    <t>tax_prd</t>
-  </si>
-  <si>
-    <t>tax_prd_yr</t>
-  </si>
-  <si>
-    <t>totcntrbgfts</t>
-  </si>
-  <si>
-    <t>totprgmrevnue</t>
-  </si>
-  <si>
-    <t>invstmntinc</t>
-  </si>
-  <si>
-    <t>FilingVar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -738,31 +767,35 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>83</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>82</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>87</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="17">
         <v>42103580</v>
       </c>
@@ -770,16 +803,19 @@
         <v>2001</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>5</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>93</v>
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="17">
         <v>60646973</v>
       </c>
@@ -787,119 +823,146 @@
         <v>2002</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>8</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>94</v>
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="12"/>
       <c r="B4" s="18">
         <f>+B3+1</f>
         <v>2003</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>12</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>95</v>
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="12"/>
       <c r="B5" s="18">
         <f t="shared" ref="B5:B21" si="0">+B4+1</f>
         <v>2004</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>96</v>
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="12"/>
       <c r="B6" s="18">
         <f t="shared" si="0"/>
         <v>2005</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>20</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>97</v>
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="12"/>
       <c r="B7" s="18">
         <f t="shared" si="0"/>
         <v>2006</v>
       </c>
       <c r="D7" s="12"/>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
       <c r="F7" s="18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="12"/>
       <c r="B8" s="18">
         <f t="shared" si="0"/>
         <v>2007</v>
       </c>
       <c r="D8" s="12"/>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
       <c r="F8" s="18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="12"/>
       <c r="B9" s="18">
         <f t="shared" si="0"/>
         <v>2008</v>
       </c>
       <c r="D9" s="12"/>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
       <c r="F9" s="18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="12"/>
       <c r="B10" s="18">
         <f t="shared" si="0"/>
         <v>2009</v>
       </c>
       <c r="D10" s="12"/>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
       <c r="F10" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="12"/>
       <c r="B11" s="18">
         <f t="shared" si="0"/>
         <v>2010</v>
       </c>
       <c r="D11" s="12"/>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
       <c r="F11" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="12"/>
       <c r="B12" s="18">
         <f t="shared" si="0"/>
@@ -907,10 +970,10 @@
       </c>
       <c r="D12" s="12"/>
       <c r="F12" s="18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="12"/>
       <c r="B13" s="18">
         <f t="shared" si="0"/>
@@ -918,10 +981,10 @@
       </c>
       <c r="D13" s="12"/>
       <c r="F13" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="12"/>
       <c r="B14" s="18">
         <f t="shared" si="0"/>
@@ -929,10 +992,10 @@
       </c>
       <c r="D14" s="12"/>
       <c r="F14" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="12"/>
       <c r="B15" s="18">
         <f t="shared" si="0"/>
@@ -940,10 +1003,10 @@
       </c>
       <c r="D15" s="12"/>
       <c r="F15" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="12"/>
       <c r="B16" s="18">
         <f t="shared" si="0"/>
@@ -951,10 +1014,10 @@
       </c>
       <c r="D16" s="12"/>
       <c r="F16" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="12"/>
       <c r="B17" s="18">
         <f t="shared" si="0"/>
@@ -962,10 +1025,10 @@
       </c>
       <c r="D17" s="12"/>
       <c r="F17" s="18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="12"/>
       <c r="B18" s="18">
         <f t="shared" si="0"/>
@@ -973,10 +1036,10 @@
       </c>
       <c r="D18" s="12"/>
       <c r="F18" s="18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="12"/>
       <c r="B19" s="18">
         <f t="shared" si="0"/>
@@ -984,10 +1047,10 @@
       </c>
       <c r="D19" s="12"/>
       <c r="F19" s="18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="12"/>
       <c r="B20" s="18">
         <f t="shared" si="0"/>
@@ -995,10 +1058,10 @@
       </c>
       <c r="D20" s="12"/>
       <c r="F20" s="18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="12"/>
       <c r="B21" s="18">
         <f t="shared" si="0"/>
@@ -1006,127 +1069,127 @@
       </c>
       <c r="D21" s="12"/>
       <c r="F21" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="D22" s="12"/>
       <c r="F22" s="18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="12"/>
       <c r="B23" s="12"/>
       <c r="D23" s="12"/>
       <c r="F23" s="18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="D24" s="12"/>
       <c r="F24" s="18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
       <c r="D25" s="12"/>
       <c r="F25" s="18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="12"/>
       <c r="B26" s="12"/>
       <c r="D26" s="12"/>
       <c r="F26" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="D27" s="12"/>
       <c r="F27" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
       <c r="D28" s="12"/>
       <c r="F28" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="D29" s="12"/>
       <c r="F29" s="18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
       <c r="D30" s="12"/>
       <c r="F30" s="18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="12"/>
       <c r="B31" s="12"/>
       <c r="D31" s="12"/>
       <c r="F31" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="12"/>
       <c r="B32" s="12"/>
       <c r="D32" s="12"/>
       <c r="F32" s="18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="12"/>
       <c r="B33" s="12"/>
       <c r="D33" s="12"/>
       <c r="F33" s="18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="12"/>
       <c r="B34" s="12"/>
       <c r="D34" s="12"/>
       <c r="F34" s="18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="12"/>
       <c r="B35" s="12"/>
       <c r="D35" s="12"/>
       <c r="F35" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="12"/>
       <c r="B36" s="12"/>
       <c r="D36" s="12"/>
       <c r="F36" s="18" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1139,11 +1202,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AJ12"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
@@ -1152,9 +1215,11 @@
     <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.28515625" customWidth="1"/>
+    <col min="14" max="14" width="17" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15.140625" customWidth="1"/>
     <col min="21" max="21" width="14.28515625" customWidth="1"/>
@@ -1163,43 +1228,43 @@
     <col min="29" max="29" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36">
       <c r="A1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36">
       <c r="A2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36">
       <c r="B3" s="5" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="7" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="7" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="7" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="10" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="Q3" s="11"/>
       <c r="R3" s="11"/>
@@ -1207,21 +1272,21 @@
       <c r="T3" s="11"/>
       <c r="U3" s="11"/>
       <c r="V3" s="10" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="W3" s="11"/>
       <c r="X3" s="11"/>
       <c r="Y3" s="11"/>
       <c r="Z3" s="11"/>
       <c r="AA3" s="10" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="AB3" s="11"/>
       <c r="AC3" s="10" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="AD3" s="10" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="AE3" s="11"/>
       <c r="AF3" s="11"/>
@@ -1230,119 +1295,119 @@
       <c r="AI3" s="11"/>
       <c r="AJ3" s="11"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="V4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="AB4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC4" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="AD4" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="AF4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="AG4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="AH4" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="AI4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="AJ4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="P4" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="V4" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="X4" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y4" s="4" t="s">
+    </row>
+    <row r="5" spans="1:36">
+      <c r="A5" t="s">
         <v>68</v>
-      </c>
-      <c r="Z4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA4" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB4" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AC4" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="AD4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ4" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>81</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1365,19 +1430,19 @@
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
       <c r="V5" s="8" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="X5" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="Z5" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="AA5" s="8"/>
       <c r="AB5" s="4"/>
@@ -1390,125 +1455,125 @@
       <c r="AI5" s="4"/>
       <c r="AJ5" s="4"/>
     </row>
-    <row r="6" spans="1:36" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" ht="54.75" customHeight="1">
       <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>4</v>
-      </c>
       <c r="G6" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="H6" s="9" t="s">
-        <v>5</v>
-      </c>
       <c r="I6" s="6" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>7</v>
+        <v>78</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="P6" s="9" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>12</v>
+        <v>85</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="T6" s="6" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>16</v>
+        <v>89</v>
       </c>
       <c r="V6" s="9" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="W6" s="6" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="X6" s="6" t="s">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="Y6" s="6" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="Z6" s="6" t="s">
-        <v>26</v>
+        <v>94</v>
       </c>
       <c r="AA6" s="9" t="s">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="AB6" s="6" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="AC6" s="9" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="AD6" s="9" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="AE6" s="6" t="s">
-        <v>32</v>
+        <v>99</v>
       </c>
       <c r="AF6" s="6" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="AG6" s="6" t="s">
-        <v>34</v>
+        <v>101</v>
       </c>
       <c r="AH6" s="6" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="AI6" s="6" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="AJ6" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="B7" s="12">
         <v>42103580</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="13">
@@ -1608,19 +1673,19 @@
         <v>38047626000</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36">
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36">
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36">
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36">
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36">
       <c r="C12" s="1"/>
     </row>
   </sheetData>
@@ -1639,11 +1704,11 @@
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>